<commit_message>
Update app and error messages
</commit_message>
<xml_diff>
--- a/DataCheckingErrorCodes.xlsx
+++ b/DataCheckingErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED8FD63-3BC9-47A0-B41E-5FE4CA7480F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E65FBE5-C330-4C82-A4EC-F3F23F953867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4719E786-03FF-A74D-9C1B-55BF7F93C6FF}"/>
+    <workbookView xWindow="12960" yWindow="1080" windowWidth="16185" windowHeight="11385" xr2:uid="{4719E786-03FF-A74D-9C1B-55BF7F93C6FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
   <si>
     <t>F01</t>
   </si>
@@ -81,9 +81,6 @@
     <t>F16</t>
   </si>
   <si>
-    <t>F17</t>
-  </si>
-  <si>
     <t>ErrorCode</t>
   </si>
   <si>
@@ -147,21 +144,12 @@
     <t>ORV issue</t>
   </si>
   <si>
-    <t>You have entered a LASTORV, but NAIVE = “YES”</t>
-  </si>
-  <si>
-    <t>The BAIT you entered doesn’t match the ORV shapefile; please check your records</t>
-  </si>
-  <si>
     <t>A record with this ANIMALID on this DATECOLLCT already exists</t>
   </si>
   <si>
     <t>F18</t>
   </si>
   <si>
-    <t>The animal was caught in the last 30 days but PROCESSED&lt;30DAYSAGE = “NO”</t>
-  </si>
-  <si>
     <t>Unique individual issue</t>
   </si>
   <si>
@@ -183,15 +171,9 @@
     <t>F21</t>
   </si>
   <si>
-    <t>It has been more than 365 days since DATE and no AGE results are entered. Please enter AGE results</t>
-  </si>
-  <si>
     <t>Age issue</t>
   </si>
   <si>
-    <t>It has been more than 365 days since DATE and RABIESBRAINTEST is “NOT RECORDED”. Please change to “YES” or “NO”. If “NO”, indicate why in the COMMENTS</t>
-  </si>
-  <si>
     <t>F22</t>
   </si>
   <si>
@@ -201,9 +183,6 @@
     <t>F23</t>
   </si>
   <si>
-    <t>It has been more than 365 days since DATE and no RABIESVNA_IUML results are entered. Please enter RABIESVNA_IUML results</t>
-  </si>
-  <si>
     <t>Rabies titer issue</t>
   </si>
   <si>
@@ -216,9 +195,6 @@
     <t>F25</t>
   </si>
   <si>
-    <t>When BLOODSAMPLE is “YES”, RABIESSERUM must be “YES” or there must be a note in COMMENTS explaining</t>
-  </si>
-  <si>
     <t>Rabies serum issue</t>
   </si>
   <si>
@@ -322,6 +298,60 @@
   </si>
   <si>
     <t>If METHOD is "CAGE TRAP" then FATE must be "'DIED UNDER CARE" or "EUTHANIZED" or "FOUND DEAD" or "OTHER" or "RELEASED" or "NO FATE"</t>
+  </si>
+  <si>
+    <t>The animal was caught in the last 30 days but PROCESSED&lt;30DAYSAGO = “NO”</t>
+  </si>
+  <si>
+    <t>It has been more than 30 days since DATE and RABIESBRAINTEST is “NOT RECORDED”. Please change RABIESBRAINTEST to “YES” or “NO”. If “NO”, indicate why in the COMMENTS</t>
+  </si>
+  <si>
+    <t>F23b</t>
+  </si>
+  <si>
+    <t>Rabies variant issue</t>
+  </si>
+  <si>
+    <t>You have entered a LASTORV, but ORVNAIVE = “YES”</t>
+  </si>
+  <si>
+    <t>It has been more than 365 days since a tooth sample was collected and there are no AGE results entered and AGERECORDED does not equal “NO”. Please enter AGE results.</t>
+  </si>
+  <si>
+    <t>F19b</t>
+  </si>
+  <si>
+    <t>Sex issue</t>
+  </si>
+  <si>
+    <t>If an animal is lactating it must be a female, check LATATION and SEX</t>
+  </si>
+  <si>
+    <t>When BLOODSAMPLE is “YES”, RABIESSERUM must be “YES” or if “NO”, indicate why in the COMMENTS.</t>
+  </si>
+  <si>
+    <t>A blood sample was taken but it has been more than 365 days since collection and no RABIESVNA_IUML results are entered. Please enter RABIESVNA_IUML results.</t>
+  </si>
+  <si>
+    <t>RABIESBRAINRESULTS is "POSITIVE" but RABIESVARIANT is "AWAITING VARIANT TYPING" and it has been more than 30 days, the variant type should be updated</t>
+  </si>
+  <si>
+    <t>F37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If TARGETSPECIES is “YES” the SPECIES must be a target species for the NRMP unless the animal was euthanized then it can be a different species. </t>
+  </si>
+  <si>
+    <t>Species issue</t>
+  </si>
+  <si>
+    <t>F38</t>
+  </si>
+  <si>
+    <t>Make sure the RABIESVNA_IUML value and the RABIESVNAINTERPRET value agree</t>
+  </si>
+  <si>
+    <t>VNA results issue</t>
   </si>
 </sst>
 </file>
@@ -439,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -464,6 +494,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B3A3A7-3EC3-9D46-96E1-CC6A3D1B7814}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -793,16 +831,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -810,10 +848,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -821,10 +859,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -832,10 +870,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -843,10 +881,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -854,39 +892,43 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -894,10 +936,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -905,10 +947,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -916,10 +958,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -927,10 +969,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -938,10 +980,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -949,10 +991,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -960,10 +1002,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -971,10 +1013,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -982,21 +1024,21 @@
         <v>14</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1004,210 +1046,243 @@
         <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>84</v>
+        <v>72</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>22</v>
+    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update app and error codes
</commit_message>
<xml_diff>
--- a/DataCheckingErrorCodes.xlsx
+++ b/DataCheckingErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E65FBE5-C330-4C82-A4EC-F3F23F953867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DEF9FA-EC67-4F3B-B325-614EE6508273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="1080" windowWidth="16185" windowHeight="11385" xr2:uid="{4719E786-03FF-A74D-9C1B-55BF7F93C6FF}"/>
+    <workbookView xWindow="15150" yWindow="735" windowWidth="13650" windowHeight="11385" xr2:uid="{4719E786-03FF-A74D-9C1B-55BF7F93C6FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,9 +339,6 @@
     <t>F37</t>
   </si>
   <si>
-    <t xml:space="preserve">If TARGETSPECIES is “YES” the SPECIES must be a target species for the NRMP unless the animal was euthanized then it can be a different species. </t>
-  </si>
-  <si>
     <t>Species issue</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>VNA results issue</t>
+  </si>
+  <si>
+    <t>NRMP target animals are: bobcats, coyotes, foxes, raccoons and skunks.  You have a mismatch between the SPECIES and TARGETSPECIES fields.  Please check to make sure your values are correct for these fields and edit MIS if they are not.</t>
   </si>
 </sst>
 </file>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B3A3A7-3EC3-9D46-96E1-CC6A3D1B7814}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1263,26 +1263,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>101</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="C41" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>